<commit_message>
district level crawling, transform html to .xlsx
</commit_message>
<xml_diff>
--- a/Mexico/input.xlsx
+++ b/Mexico/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\crops\crawler\Mexico\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB533F55-6952-4FF5-B73A-B2A8549B5999}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0AE8328-B125-4E26-8330-EB993485F8A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1476" yWindow="1997" windowWidth="17426" windowHeight="9039" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6692" yWindow="1089" windowWidth="17425" windowHeight="9039" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Year</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -35,22 +35,22 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>State</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>District</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Baja California</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Elote</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>State</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>District</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Municipio</t>
-  </si>
-  <si>
-    <t>Guanajuato</t>
+  </si>
+  <si>
+    <t>Municipality</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -58,7 +58,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,6 +68,13 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
@@ -94,8 +101,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -376,10 +384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScale="104" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.95" x14ac:dyDescent="0.25"/>
@@ -390,13 +398,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -407,21 +415,14 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="B2" s="1"/>
       <c r="D2">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="E2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D3">
-        <v>2021</v>
-      </c>
-      <c r="E3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rearrange data, add servive
</commit_message>
<xml_diff>
--- a/Mexico/input.xlsx
+++ b/Mexico/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\crops\crawler\Mexico\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0AE8328-B125-4E26-8330-EB993485F8A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4082F976-027A-4156-89B2-7E4ACB542628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6692" yWindow="1089" windowWidth="17425" windowHeight="9039" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2626" yWindow="2626" windowWidth="17425" windowHeight="9039" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Year</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -40,10 +40,6 @@
   </si>
   <si>
     <t>District</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Baja California</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -387,7 +383,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="104" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.95" x14ac:dyDescent="0.25"/>
@@ -404,7 +400,7 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -414,15 +410,12 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
       <c r="B2" s="1"/>
       <c r="D2">
         <v>2021</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adjust sub-district cralwing method
</commit_message>
<xml_diff>
--- a/Mexico/input.xlsx
+++ b/Mexico/input.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,525 +453,210 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Nacional</t>
+          <t>Sub</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1988</v>
+        <v>2009</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Mostaza</t>
+          <t>Maíz grano</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Nacional</t>
+          <t>Sub</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1989</v>
+        <v>2010</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Mostaza</t>
+          <t>Maíz grano</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Nacional</t>
+          <t>Sub</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1990</v>
+        <v>2011</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Mostaza</t>
+          <t>Maíz grano</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Nacional</t>
+          <t>Sub</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1991</v>
+        <v>2012</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Mostaza</t>
+          <t>Maíz grano</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Nacional</t>
+          <t>Sub</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1992</v>
+        <v>2013</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Mostaza</t>
+          <t>Maíz grano</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Nacional</t>
+          <t>Sub</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1993</v>
+        <v>2014</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Mostaza</t>
+          <t>Maíz grano</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Nacional</t>
+          <t>Sub</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1994</v>
+        <v>2015</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Mostaza</t>
+          <t>Maíz grano</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Nacional</t>
+          <t>Sub</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1995</v>
+        <v>2016</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Mostaza</t>
+          <t>Maíz grano</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Nacional</t>
+          <t>Sub</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1996</v>
+        <v>2017</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Mostaza</t>
+          <t>Maíz grano</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Nacional</t>
+          <t>Sub</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1997</v>
+        <v>2018</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Mostaza</t>
+          <t>Maíz grano</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Nacional</t>
+          <t>Sub</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1998</v>
+        <v>2019</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Mostaza</t>
+          <t>Maíz grano</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Nacional</t>
+          <t>Sub</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1999</v>
+        <v>2020</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Mostaza</t>
+          <t>Maíz grano</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Nacional</t>
+          <t>Sub</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>2000</v>
+        <v>2021</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Mostaza</t>
+          <t>Maíz grano</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Nacional</t>
+          <t>Sub</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>2001</v>
+        <v>2022</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Mostaza</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Nacional</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>2002</v>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Mostaza</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Nacional</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>2003</v>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Mostaza</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Nacional</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>2004</v>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Mostaza</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Nacional</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>2005</v>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Mostaza</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Nacional</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>2006</v>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Mostaza</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Nacional</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>2007</v>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Mostaza</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Nacional</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>2008</v>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>Mostaza</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Nacional</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>2009</v>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Mostaza</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Nacional</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>2010</v>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>Mostaza</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>Nacional</t>
-        </is>
-      </c>
-      <c r="B25" t="n">
-        <v>2011</v>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Mostaza</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>Nacional</t>
-        </is>
-      </c>
-      <c r="B26" t="n">
-        <v>2012</v>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>Mostaza</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>Nacional</t>
-        </is>
-      </c>
-      <c r="B27" t="n">
-        <v>2013</v>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>Mostaza</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>Nacional</t>
-        </is>
-      </c>
-      <c r="B28" t="n">
-        <v>2014</v>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>Mostaza</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>Nacional</t>
-        </is>
-      </c>
-      <c r="B29" t="n">
-        <v>2015</v>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>Mostaza</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>Nacional</t>
-        </is>
-      </c>
-      <c r="B30" t="n">
-        <v>2016</v>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>Mostaza</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>Nacional</t>
-        </is>
-      </c>
-      <c r="B31" t="n">
-        <v>2017</v>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>Mostaza</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>Nacional</t>
-        </is>
-      </c>
-      <c r="B32" t="n">
-        <v>2018</v>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>Mostaza</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>Nacional</t>
-        </is>
-      </c>
-      <c r="B33" t="n">
-        <v>2019</v>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>Mostaza</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>Nacional</t>
-        </is>
-      </c>
-      <c r="B34" t="n">
-        <v>2020</v>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>Mostaza</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>Nacional</t>
-        </is>
-      </c>
-      <c r="B35" t="n">
-        <v>2021</v>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>Mostaza</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>Nacional</t>
-        </is>
-      </c>
-      <c r="B36" t="n">
-        <v>2022</v>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>Mostaza</t>
+          <t>Maíz grano</t>
         </is>
       </c>
     </row>

</xml_diff>